<commit_message>
negative power is now zero
</commit_message>
<xml_diff>
--- a/analyse/output.xlsx
+++ b/analyse/output.xlsx
@@ -523,7 +523,7 @@
         <v>62.06</v>
       </c>
       <c r="H3" t="n">
-        <v>-39.36</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -551,7 +551,7 @@
         <v>70.16</v>
       </c>
       <c r="H4" t="n">
-        <v>-70.14</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -579,7 +579,7 @@
         <v>54</v>
       </c>
       <c r="H5" t="n">
-        <v>-67.66</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -607,7 +607,7 @@
         <v>99.75</v>
       </c>
       <c r="H6" t="n">
-        <v>-67.22</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>